<commit_message>
repex for mutate function
</commit_message>
<xml_diff>
--- a/INPUT-FILES/OES-TABLES/Form-Agestrat-CV.xlsx
+++ b/INPUT-FILES/OES-TABLES/Form-Agestrat-CV.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dherzberg/Desktop/R/DP4-R/INPUT-FILES/OES-TABLES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1EE2E5F9-2409-1748-B858-6D4CB9CBEFA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E409E087-2235-5C40-AF5A-709C8059E354}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1160" yWindow="1060" windowWidth="27640" windowHeight="16940" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25600" yWindow="460" windowWidth="25600" windowHeight="28340" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Interview-CV90" sheetId="1" r:id="rId1"/>
@@ -1627,8 +1627,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1672,6 +1672,9 @@
       <c r="E2" s="1">
         <v>10</v>
       </c>
+      <c r="F2">
+        <v>14</v>
+      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -1689,6 +1692,9 @@
       <c r="E3" s="1">
         <v>10</v>
       </c>
+      <c r="F3">
+        <v>14</v>
+      </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1706,6 +1712,9 @@
       <c r="E4" s="1">
         <v>10</v>
       </c>
+      <c r="F4">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -1723,6 +1732,9 @@
       <c r="E5" s="1">
         <v>10</v>
       </c>
+      <c r="F5">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1740,6 +1752,9 @@
       <c r="E6" s="1">
         <v>10</v>
       </c>
+      <c r="F6">
+        <v>14</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
@@ -1757,6 +1772,9 @@
       <c r="E7" s="1">
         <v>10</v>
       </c>
+      <c r="F7">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
@@ -1774,6 +1792,9 @@
       <c r="E8" s="1">
         <v>13</v>
       </c>
+      <c r="F8">
+        <v>17</v>
+      </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
@@ -1791,6 +1812,9 @@
       <c r="E9" s="1">
         <v>13</v>
       </c>
+      <c r="F9">
+        <v>17</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
@@ -1808,6 +1832,9 @@
       <c r="E10" s="1">
         <v>13</v>
       </c>
+      <c r="F10">
+        <v>17</v>
+      </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
@@ -1825,6 +1852,9 @@
       <c r="E11" s="1">
         <v>13</v>
       </c>
+      <c r="F11">
+        <v>17</v>
+      </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
@@ -1842,6 +1872,9 @@
       <c r="E12" s="1">
         <v>13</v>
       </c>
+      <c r="F12">
+        <v>17</v>
+      </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
@@ -1859,6 +1892,9 @@
       <c r="E13" s="1">
         <v>13</v>
       </c>
+      <c r="F13">
+        <v>17</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
@@ -1876,6 +1912,9 @@
       <c r="E14" s="1">
         <v>14</v>
       </c>
+      <c r="F14">
+        <v>14</v>
+      </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
@@ -1893,6 +1932,9 @@
       <c r="E15" s="1">
         <v>14</v>
       </c>
+      <c r="F15">
+        <v>14</v>
+      </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
@@ -1910,8 +1952,11 @@
       <c r="E16" s="1">
         <v>14</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>9</v>
       </c>
@@ -1927,8 +1972,11 @@
       <c r="E17" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>10</v>
       </c>
@@ -1944,8 +1992,11 @@
       <c r="E18" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>11</v>
       </c>
@@ -1961,8 +2012,11 @@
       <c r="E19" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>12</v>
       </c>
@@ -1978,8 +2032,11 @@
       <c r="E20" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>13</v>
       </c>
@@ -1995,8 +2052,11 @@
       <c r="E21" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>14</v>
       </c>
@@ -2012,8 +2072,11 @@
       <c r="E22" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>15</v>
       </c>
@@ -2029,8 +2092,11 @@
       <c r="E23" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>16</v>
       </c>
@@ -2046,8 +2112,11 @@
       <c r="E24" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>17</v>
       </c>
@@ -2063,8 +2132,11 @@
       <c r="E25" s="1">
         <v>12</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>18</v>
       </c>
@@ -2080,8 +2152,11 @@
       <c r="E26" s="1">
         <v>11</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>19</v>
       </c>
@@ -2097,8 +2172,11 @@
       <c r="E27" s="1">
         <v>10</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>20</v>
       </c>
@@ -2114,8 +2192,11 @@
       <c r="E28" s="1">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>21</v>
       </c>
@@ -2131,8 +2212,11 @@
       <c r="E29" s="1">
         <v>13</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>22</v>
       </c>
@@ -2148,8 +2232,11 @@
       <c r="E30" s="1">
         <v>8</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>23</v>
       </c>
@@ -2164,6 +2251,9 @@
       </c>
       <c r="E31" s="1">
         <v>9</v>
+      </c>
+      <c r="F31">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -3849,7 +3939,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AD36"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+    <sheetView zoomScale="112" workbookViewId="0">
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>